<commit_message>
Modified data analysis slightly
</commit_message>
<xml_diff>
--- a/Testing/Ash Chamber Sensor Testing/Testing 29 Aug/OPC and PMS Chamber testing 29Aug.xlsx
+++ b/Testing/Ash Chamber Sensor Testing/Testing 29 Aug/OPC and PMS Chamber testing 29Aug.xlsx
@@ -12346,10 +12346,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="40000"/>
-                  <a:lumOff val="60000"/>
-                </a:schemeClr>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -20941,7 +20938,7 @@
   <dimension ref="A1:T1223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>